<commit_message>
Deploy wizard + BALTA template
</commit_message>
<xml_diff>
--- a/docs/templates/balta_template.xlsx
+++ b/docs/templates/balta_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10824"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dainis Samuilovs\Documents\tāmes\2024\08\1284332 Parka iela 14, Jelgava\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gabriellakonstantinova/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{515C70FB-321E-4D37-9C00-81DF1DADB2DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{44742078-E2B9-7E4F-9EC8-BFD479674187}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="817" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" tabRatio="817" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tāme" sheetId="26" r:id="rId1"/>
@@ -20,7 +20,20 @@
     <definedName name="kurss">#REF!</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Tāme!$A$1:$L$84</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -61,7 +74,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="45">
   <si>
     <t>Darba nosaukums</t>
   </si>
@@ -78,9 +91,6 @@
     <t xml:space="preserve"> AAS Balta</t>
   </si>
   <si>
-    <t>m</t>
-  </si>
-  <si>
     <t>Mērvienība</t>
   </si>
   <si>
@@ -94,12 +104,6 @@
   </si>
   <si>
     <t>Kopā uz visu apjomu</t>
-  </si>
-  <si>
-    <t>m2</t>
-  </si>
-  <si>
-    <t>l</t>
   </si>
   <si>
     <t xml:space="preserve">Kopā </t>
@@ -186,19 +190,7 @@
     <t>Pavisam kopā</t>
   </si>
   <si>
-    <t>c/h</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Tiešās izmaksas kopā</t>
-  </si>
-  <si>
-    <t>m3</t>
-  </si>
-  <si>
-    <t>kpl.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">grunts </t>
   </si>
   <si>
     <t>Materiālu, grunts apmaiņas un būvgružu transporta izdevumi</t>
@@ -211,9 +203,6 @@
   </si>
   <si>
     <t> Peļņa</t>
-  </si>
-  <si>
-    <t>Mēbeļu demontāža, parvietošana, montāža</t>
   </si>
   <si>
     <t>Piezīmes:</t>
@@ -304,54 +293,6 @@
     </r>
   </si>
   <si>
-    <t>Telpu uzkopšana pēc remonta darbu pabeigšanas</t>
-  </si>
-  <si>
-    <t>Būvgružu savākšana un izvešana</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Telpu sagatavošana remontdarbiem </t>
-  </si>
-  <si>
-    <t>Sienu attīrīšana no esošā seguma</t>
-  </si>
-  <si>
-    <t>Tapešu līmēšana uz sienām</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> tapetes (vidējā cena)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tapešu līme  </t>
-  </si>
-  <si>
-    <t>Grīdas seguma demontāža (lamināts)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lamināta apakšklāja montāža  </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> kokšķiedras izolācijas plātnes , 5mm</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lamināta ieklāšana </t>
-  </si>
-  <si>
-    <t>lamināts (vidējā cena)</t>
-  </si>
-  <si>
-    <t>PVC grīdlīstes montāža</t>
-  </si>
-  <si>
-    <t>dībeļnagla 6x50mm</t>
-  </si>
-  <si>
-    <t>100gb.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PVC plastmasas grīdlīste </t>
-  </si>
-  <si>
     <t>Objekts: dzīvojama māja</t>
   </si>
   <si>
@@ -392,102 +333,6 @@
       </rPr>
       <t>, objekta fotofiksācija, nekustamā īpašuma apsekošanas akts</t>
     </r>
-  </si>
-  <si>
-    <t>gaitenis nr.14</t>
-  </si>
-  <si>
-    <t>istaba nr. 18</t>
-  </si>
-  <si>
-    <t>Griestu attīrīšana no esošā seguma</t>
-  </si>
-  <si>
-    <t>Regipša griestu sagatavošana apdarei sausās telpās (gruntēšana,špaktelēšana,slīpēšana)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">špaktele </t>
-  </si>
-  <si>
-    <t>kg</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> gatavā smalkā špaktele </t>
-  </si>
-  <si>
-    <t>sietiņlenta</t>
-  </si>
-  <si>
-    <t>45m</t>
-  </si>
-  <si>
-    <t xml:space="preserve">reģipša šuvju špaktele </t>
-  </si>
-  <si>
-    <t>smilšpapīrs,krāsotāju līmlenta</t>
-  </si>
-  <si>
-    <t>Griestu gruntēšana un krāsošana divos slāņos</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ūdens emulsijas grunts krāsa </t>
-  </si>
-  <si>
-    <t>ūdens emulsijas krāsa , balta</t>
-  </si>
-  <si>
-    <t>Jumts</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jumta seguma demontāža </t>
-  </si>
-  <si>
-    <t>Jumta nesošās konstrukciju remonts</t>
-  </si>
-  <si>
-    <t>kpl</t>
-  </si>
-  <si>
-    <t>Jumta esošo seguma montaža</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Alumīnija torņa  montāža,demontāža, noma - </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="9"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="186"/>
-      </rPr>
-      <t>h=6m-12m</t>
-    </r>
-  </si>
-  <si>
-    <t>diena</t>
-  </si>
-  <si>
-    <t>Jumta seguma montaža</t>
-  </si>
-  <si>
-    <t>Garaža</t>
-  </si>
-  <si>
-    <t>Preskartona montāža</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> - preskartons 3mm</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> - palīgmateriāli</t>
-  </si>
-  <si>
-    <t>Gaismekļu, rozešu un slēdžu demontāža, montāža un pieslēgšana</t>
-  </si>
-  <si>
-    <t>gb.</t>
   </si>
   <si>
     <t>Rīga, 2024. gada 2.oktobris</t>
@@ -1136,6 +981,45 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="2" xfId="28" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="2" xfId="32" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="9" fillId="6" borderId="2" xfId="32" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="9" fillId="6" borderId="2" xfId="32" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="9" fillId="6" borderId="2" xfId="30" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="15" fillId="6" borderId="2" xfId="29" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="9" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="9" fillId="6" borderId="2" xfId="30" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="9" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="9" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="17" fillId="4" borderId="2" xfId="26" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1147,45 +1031,6 @@
     </xf>
     <xf numFmtId="0" fontId="17" fillId="4" borderId="2" xfId="26" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="2" xfId="28" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="2" xfId="32" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="9" fillId="6" borderId="2" xfId="32" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="9" fillId="6" borderId="2" xfId="32" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="9" fillId="6" borderId="2" xfId="30" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="15" fillId="6" borderId="2" xfId="29" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="9" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="9" fillId="6" borderId="2" xfId="30" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="9" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="9" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="41">
@@ -4286,34 +4131,34 @@
   </sheetPr>
   <dimension ref="A1:R84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A65" zoomScale="111" zoomScaleNormal="111" workbookViewId="0">
-      <selection activeCell="B79" sqref="B79"/>
+    <sheetView tabSelected="1" zoomScale="111" zoomScaleNormal="111" workbookViewId="0">
+      <selection activeCell="J66" sqref="J66"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="4.5703125" style="25" customWidth="1"/>
-    <col min="2" max="2" width="52.42578125" style="26" customWidth="1"/>
+    <col min="1" max="1" width="4.5" style="25" customWidth="1"/>
+    <col min="2" max="2" width="52.5" style="26" customWidth="1"/>
     <col min="3" max="3" width="9" style="26" customWidth="1"/>
-    <col min="4" max="4" width="9.42578125" style="26" customWidth="1"/>
-    <col min="5" max="5" width="8.7109375" style="26" customWidth="1"/>
-    <col min="6" max="6" width="9.85546875" style="26" customWidth="1"/>
-    <col min="7" max="7" width="9.140625" style="26" customWidth="1"/>
-    <col min="8" max="8" width="10.7109375" style="26" customWidth="1"/>
-    <col min="9" max="9" width="10.42578125" style="6" customWidth="1"/>
-    <col min="10" max="10" width="11.140625" style="6" customWidth="1"/>
-    <col min="11" max="11" width="9.7109375" style="6" customWidth="1"/>
-    <col min="12" max="12" width="12.140625" style="6" customWidth="1"/>
+    <col min="4" max="4" width="9.5" style="26" customWidth="1"/>
+    <col min="5" max="5" width="8.6640625" style="26" customWidth="1"/>
+    <col min="6" max="6" width="9.83203125" style="26" customWidth="1"/>
+    <col min="7" max="7" width="9.1640625" style="26" customWidth="1"/>
+    <col min="8" max="8" width="10.6640625" style="26" customWidth="1"/>
+    <col min="9" max="9" width="10.5" style="6" customWidth="1"/>
+    <col min="10" max="10" width="11.1640625" style="6" customWidth="1"/>
+    <col min="11" max="11" width="9.6640625" style="6" customWidth="1"/>
+    <col min="12" max="12" width="12.1640625" style="6" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" s="30" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B1" s="31"/>
       <c r="C1" s="31"/>
       <c r="D1" s="32" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="E1" s="33"/>
       <c r="F1" s="34"/>
@@ -4325,12 +4170,12 @@
     </row>
     <row r="2" spans="1:12">
       <c r="A2" s="32" t="s">
-        <v>63</v>
+        <v>39</v>
       </c>
       <c r="B2" s="31"/>
       <c r="C2" s="31"/>
       <c r="D2" s="32" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="E2" s="35"/>
       <c r="F2" s="35"/>
@@ -4342,12 +4187,12 @@
     </row>
     <row r="3" spans="1:12">
       <c r="A3" s="32" t="s">
-        <v>64</v>
+        <v>40</v>
       </c>
       <c r="B3" s="31"/>
       <c r="C3" s="31"/>
       <c r="D3" s="32" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="E3" s="35"/>
       <c r="F3" s="35"/>
@@ -4370,21 +4215,21 @@
       <c r="J4" s="31"/>
       <c r="K4" s="31"/>
     </row>
-    <row r="5" spans="1:12" ht="15.75">
-      <c r="A5" s="112" t="s">
-        <v>95</v>
-      </c>
-      <c r="B5" s="112"/>
-      <c r="C5" s="112"/>
-      <c r="D5" s="112"/>
-      <c r="E5" s="112"/>
-      <c r="F5" s="112"/>
-      <c r="G5" s="112"/>
-      <c r="H5" s="112"/>
-      <c r="I5" s="112"/>
-      <c r="J5" s="112"/>
-      <c r="K5" s="112"/>
-      <c r="L5" s="112"/>
+    <row r="5" spans="1:12" ht="16">
+      <c r="A5" s="125" t="s">
+        <v>43</v>
+      </c>
+      <c r="B5" s="125"/>
+      <c r="C5" s="125"/>
+      <c r="D5" s="125"/>
+      <c r="E5" s="125"/>
+      <c r="F5" s="125"/>
+      <c r="G5" s="125"/>
+      <c r="H5" s="125"/>
+      <c r="I5" s="125"/>
+      <c r="J5" s="125"/>
+      <c r="K5" s="125"/>
+      <c r="L5" s="125"/>
     </row>
     <row r="6" spans="1:12" ht="8.25" customHeight="1">
       <c r="A6" s="5"/>
@@ -4401,20 +4246,20 @@
       <c r="L6" s="5"/>
     </row>
     <row r="7" spans="1:12" ht="15" customHeight="1">
-      <c r="A7" s="112" t="s">
-        <v>38</v>
-      </c>
-      <c r="B7" s="112"/>
-      <c r="C7" s="112"/>
-      <c r="D7" s="112"/>
-      <c r="E7" s="112"/>
-      <c r="F7" s="112"/>
-      <c r="G7" s="112"/>
-      <c r="H7" s="112"/>
-      <c r="I7" s="112"/>
-      <c r="J7" s="112"/>
-      <c r="K7" s="112"/>
-      <c r="L7" s="112"/>
+      <c r="A7" s="125" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" s="125"/>
+      <c r="C7" s="125"/>
+      <c r="D7" s="125"/>
+      <c r="E7" s="125"/>
+      <c r="F7" s="125"/>
+      <c r="G7" s="125"/>
+      <c r="H7" s="125"/>
+      <c r="I7" s="125"/>
+      <c r="J7" s="125"/>
+      <c r="K7" s="125"/>
+      <c r="L7" s="125"/>
     </row>
     <row r="8" spans="1:12" ht="9.75" customHeight="1">
       <c r="A8" s="1"/>
@@ -4432,7 +4277,7 @@
     </row>
     <row r="9" spans="1:12" s="37" customFormat="1" ht="13.5" customHeight="1">
       <c r="A9" s="28" t="s">
-        <v>94</v>
+        <v>42</v>
       </c>
       <c r="B9" s="28"/>
       <c r="C9" s="28"/>
@@ -4444,16 +4289,16 @@
       <c r="I9" s="39"/>
       <c r="J9" s="28"/>
       <c r="K9" s="38" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="L9" s="65">
         <f>L70</f>
-        <v>7319.8000000000011</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" s="37" customFormat="1" ht="12.75">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" s="37" customFormat="1" ht="13">
       <c r="A10" s="28" t="s">
-        <v>65</v>
+        <v>41</v>
       </c>
       <c r="B10" s="28"/>
       <c r="C10" s="28"/>
@@ -4469,7 +4314,7 @@
       </c>
       <c r="L10" s="66">
         <f>ROUND(L9*21%,2)</f>
-        <v>1537.16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:12" s="37" customFormat="1" ht="13.5" customHeight="1">
@@ -4484,11 +4329,11 @@
       <c r="I11" s="39"/>
       <c r="J11" s="28"/>
       <c r="K11" s="38" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="L11" s="65">
         <f>SUM(L9,L10)</f>
-        <v>8856.9600000000009</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:12">
@@ -4506,66 +4351,64 @@
       <c r="L12" s="10"/>
     </row>
     <row r="13" spans="1:12" ht="18.75" customHeight="1">
-      <c r="A13" s="113" t="s">
+      <c r="A13" s="126" t="s">
+        <v>7</v>
+      </c>
+      <c r="B13" s="124" t="s">
+        <v>0</v>
+      </c>
+      <c r="C13" s="127" t="s">
+        <v>5</v>
+      </c>
+      <c r="D13" s="127" t="s">
+        <v>6</v>
+      </c>
+      <c r="E13" s="124" t="s">
         <v>8</v>
       </c>
-      <c r="B13" s="111" t="s">
-        <v>0</v>
-      </c>
-      <c r="C13" s="114" t="s">
-        <v>6</v>
-      </c>
-      <c r="D13" s="114" t="s">
-        <v>7</v>
-      </c>
-      <c r="E13" s="111" t="s">
+      <c r="F13" s="124"/>
+      <c r="G13" s="124"/>
+      <c r="H13" s="124"/>
+      <c r="I13" s="124" t="s">
         <v>9</v>
       </c>
-      <c r="F13" s="111"/>
-      <c r="G13" s="111"/>
-      <c r="H13" s="111"/>
-      <c r="I13" s="111" t="s">
-        <v>10</v>
-      </c>
-      <c r="J13" s="111"/>
-      <c r="K13" s="111"/>
-      <c r="L13" s="111"/>
+      <c r="J13" s="124"/>
+      <c r="K13" s="124"/>
+      <c r="L13" s="124"/>
     </row>
     <row r="14" spans="1:12" ht="53.25" customHeight="1">
-      <c r="A14" s="113"/>
-      <c r="B14" s="111"/>
-      <c r="C14" s="114"/>
-      <c r="D14" s="114"/>
+      <c r="A14" s="126"/>
+      <c r="B14" s="124"/>
+      <c r="C14" s="127"/>
+      <c r="D14" s="127"/>
       <c r="E14" s="78" t="s">
+        <v>14</v>
+      </c>
+      <c r="F14" s="78" t="s">
+        <v>15</v>
+      </c>
+      <c r="G14" s="78" t="s">
+        <v>16</v>
+      </c>
+      <c r="H14" s="78" t="s">
         <v>17</v>
       </c>
-      <c r="F14" s="78" t="s">
+      <c r="I14" s="78" t="s">
+        <v>14</v>
+      </c>
+      <c r="J14" s="78" t="s">
+        <v>15</v>
+      </c>
+      <c r="K14" s="78" t="s">
+        <v>16</v>
+      </c>
+      <c r="L14" s="78" t="s">
         <v>18</v>
-      </c>
-      <c r="G14" s="78" t="s">
-        <v>19</v>
-      </c>
-      <c r="H14" s="78" t="s">
-        <v>20</v>
-      </c>
-      <c r="I14" s="78" t="s">
-        <v>17</v>
-      </c>
-      <c r="J14" s="78" t="s">
-        <v>18</v>
-      </c>
-      <c r="K14" s="78" t="s">
-        <v>19</v>
-      </c>
-      <c r="L14" s="78" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="15" spans="1:12">
       <c r="A15" s="79"/>
-      <c r="B15" s="58" t="s">
-        <v>67</v>
-      </c>
+      <c r="B15" s="58"/>
       <c r="C15" s="61"/>
       <c r="D15" s="59"/>
       <c r="E15" s="59"/>
@@ -4579,29 +4422,16 @@
     </row>
     <row r="16" spans="1:12">
       <c r="A16" s="63"/>
-      <c r="B16" s="96" t="s">
-        <v>50</v>
-      </c>
-      <c r="C16" s="42" t="s">
-        <v>11</v>
-      </c>
-      <c r="D16" s="97">
-        <v>39</v>
-      </c>
-      <c r="E16" s="90">
-        <v>1.6</v>
-      </c>
+      <c r="B16" s="96"/>
+      <c r="C16" s="42"/>
+      <c r="D16" s="97"/>
+      <c r="E16" s="90"/>
       <c r="F16" s="90"/>
-      <c r="G16" s="91">
-        <v>0.33</v>
-      </c>
-      <c r="H16" s="12">
-        <f>ROUND(SUM(E16:G16),2)</f>
-        <v>1.93</v>
-      </c>
+      <c r="G16" s="91"/>
+      <c r="H16" s="12"/>
       <c r="I16" s="12">
         <f t="shared" ref="I16:I20" si="0">ROUND(E16*D16,2)</f>
-        <v>62.4</v>
+        <v>0</v>
       </c>
       <c r="J16" s="12">
         <f t="shared" ref="J16:J20" si="1">ROUND(D16*F16,2)</f>
@@ -4609,39 +4439,25 @@
       </c>
       <c r="K16" s="12">
         <f t="shared" ref="K16:K20" si="2">ROUND(D16*G16,2)</f>
-        <v>12.87</v>
+        <v>0</v>
       </c>
       <c r="L16" s="12">
         <f>ROUND(SUM(I16:K16),2)</f>
-        <v>75.27</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:12">
       <c r="A17" s="63"/>
-      <c r="B17" s="16" t="s">
-        <v>51</v>
-      </c>
-      <c r="C17" s="42" t="s">
-        <v>11</v>
-      </c>
-      <c r="D17" s="62">
-        <f>D16</f>
-        <v>39</v>
-      </c>
-      <c r="E17" s="90">
-        <v>6.5</v>
-      </c>
+      <c r="B17" s="16"/>
+      <c r="C17" s="42"/>
+      <c r="D17" s="62"/>
+      <c r="E17" s="90"/>
       <c r="F17" s="51"/>
-      <c r="G17" s="91">
-        <v>0.24</v>
-      </c>
-      <c r="H17" s="12">
-        <f t="shared" ref="H17:H45" si="3">ROUND(SUM(E17:G17),2)</f>
-        <v>6.74</v>
-      </c>
+      <c r="G17" s="91"/>
+      <c r="H17" s="12"/>
       <c r="I17" s="12">
         <f t="shared" si="0"/>
-        <v>253.5</v>
+        <v>0</v>
       </c>
       <c r="J17" s="12">
         <f t="shared" si="1"/>
@@ -4649,132 +4465,94 @@
       </c>
       <c r="K17" s="12">
         <f t="shared" si="2"/>
-        <v>9.36</v>
+        <v>0</v>
       </c>
       <c r="L17" s="12">
-        <f t="shared" ref="L17:L20" si="4">ROUND(SUM(I17:K17),2)</f>
-        <v>262.86</v>
+        <f t="shared" ref="L17:L20" si="3">ROUND(SUM(I17:K17),2)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:12">
       <c r="A18" s="63"/>
-      <c r="B18" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="C18" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="D18" s="62">
-        <f>ROUND(D17*0.15,2)</f>
-        <v>5.85</v>
-      </c>
+      <c r="B18" s="13"/>
+      <c r="C18" s="14"/>
+      <c r="D18" s="62"/>
       <c r="E18" s="86"/>
-      <c r="F18" s="88">
-        <v>3.2</v>
-      </c>
+      <c r="F18" s="88"/>
       <c r="G18" s="91"/>
-      <c r="H18" s="12">
-        <f t="shared" si="3"/>
-        <v>3.2</v>
-      </c>
+      <c r="H18" s="12"/>
       <c r="I18" s="12">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="J18" s="12">
         <f t="shared" si="1"/>
-        <v>18.72</v>
+        <v>0</v>
       </c>
       <c r="K18" s="12">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="L18" s="12">
-        <f t="shared" si="4"/>
-        <v>18.72</v>
+        <f t="shared" si="3"/>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:12">
       <c r="A19" s="63"/>
-      <c r="B19" s="41" t="s">
-        <v>52</v>
-      </c>
-      <c r="C19" s="42" t="s">
-        <v>11</v>
-      </c>
-      <c r="D19" s="98">
-        <f>CEILING(D17*1.4,5)</f>
-        <v>55</v>
-      </c>
+      <c r="B19" s="41"/>
+      <c r="C19" s="42"/>
+      <c r="D19" s="98"/>
       <c r="E19" s="86"/>
-      <c r="F19" s="92">
-        <v>2.75</v>
-      </c>
+      <c r="F19" s="92"/>
       <c r="G19" s="91"/>
-      <c r="H19" s="12">
-        <f t="shared" si="3"/>
-        <v>2.75</v>
-      </c>
+      <c r="H19" s="12"/>
       <c r="I19" s="12">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="J19" s="12">
         <f t="shared" si="1"/>
-        <v>151.25</v>
+        <v>0</v>
       </c>
       <c r="K19" s="12">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="L19" s="12">
-        <f t="shared" si="4"/>
-        <v>151.25</v>
+        <f t="shared" si="3"/>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:12">
       <c r="A20" s="63"/>
-      <c r="B20" s="41" t="s">
-        <v>53</v>
-      </c>
-      <c r="C20" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="D20" s="62">
-        <f>ROUND(D17*0.4,2)</f>
-        <v>15.6</v>
-      </c>
+      <c r="B20" s="41"/>
+      <c r="C20" s="14"/>
+      <c r="D20" s="62"/>
       <c r="E20" s="86"/>
-      <c r="F20" s="88">
-        <v>2.5099999999999998</v>
-      </c>
+      <c r="F20" s="88"/>
       <c r="G20" s="91"/>
-      <c r="H20" s="12">
-        <f t="shared" si="3"/>
-        <v>2.5099999999999998</v>
-      </c>
+      <c r="H20" s="12"/>
       <c r="I20" s="12">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="J20" s="12">
         <f t="shared" si="1"/>
-        <v>39.159999999999997</v>
+        <v>0</v>
       </c>
       <c r="K20" s="12">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="L20" s="12">
-        <f t="shared" si="4"/>
-        <v>39.159999999999997</v>
+        <f t="shared" si="3"/>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:12">
       <c r="A21" s="79"/>
-      <c r="B21" s="58" t="s">
-        <v>66</v>
-      </c>
+      <c r="B21" s="58"/>
       <c r="C21" s="61"/>
       <c r="D21" s="59"/>
       <c r="E21" s="59"/>
@@ -4788,643 +4566,432 @@
     </row>
     <row r="22" spans="1:12">
       <c r="A22" s="63"/>
-      <c r="B22" s="102" t="s">
-        <v>68</v>
-      </c>
-      <c r="C22" s="103" t="s">
-        <v>11</v>
-      </c>
-      <c r="D22" s="103">
-        <v>1</v>
-      </c>
-      <c r="E22" s="90">
-        <v>1.6</v>
-      </c>
+      <c r="B22" s="102"/>
+      <c r="C22" s="103"/>
+      <c r="D22" s="103"/>
+      <c r="E22" s="90"/>
       <c r="F22" s="90"/>
-      <c r="G22" s="91">
-        <v>0.22</v>
-      </c>
-      <c r="H22" s="12">
-        <f t="shared" ref="H22:H32" si="5">ROUND(SUM(E22:G22),2)</f>
-        <v>1.82</v>
-      </c>
+      <c r="G22" s="91"/>
+      <c r="H22" s="12"/>
       <c r="I22" s="12">
-        <f t="shared" ref="I22:I32" si="6">ROUND(E22*D22,2)</f>
-        <v>1.6</v>
+        <f t="shared" ref="I22:I32" si="4">ROUND(E22*D22,2)</f>
+        <v>0</v>
       </c>
       <c r="J22" s="12">
-        <f t="shared" ref="J22:J32" si="7">ROUND(D22*F22,2)</f>
+        <f t="shared" ref="J22:J32" si="5">ROUND(D22*F22,2)</f>
         <v>0</v>
       </c>
       <c r="K22" s="12">
-        <f t="shared" ref="K22:K32" si="8">ROUND(D22*G22,2)</f>
-        <v>0.22</v>
+        <f t="shared" ref="K22:K32" si="6">ROUND(D22*G22,2)</f>
+        <v>0</v>
       </c>
       <c r="L22" s="12">
-        <f t="shared" ref="L22:L32" si="9">ROUND(SUM(I22:K22),2)</f>
-        <v>1.82</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" ht="24">
+        <f t="shared" ref="L22:L32" si="7">ROUND(SUM(I22:K22),2)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12">
       <c r="A23" s="63"/>
-      <c r="B23" s="16" t="s">
-        <v>69</v>
-      </c>
-      <c r="C23" s="42" t="s">
-        <v>11</v>
-      </c>
-      <c r="D23" s="62">
-        <v>1</v>
-      </c>
-      <c r="E23" s="12">
-        <v>8</v>
-      </c>
+      <c r="B23" s="16"/>
+      <c r="C23" s="42"/>
+      <c r="D23" s="62"/>
+      <c r="E23" s="12"/>
       <c r="F23" s="87"/>
-      <c r="G23" s="91">
-        <v>0.69</v>
-      </c>
-      <c r="H23" s="11">
+      <c r="G23" s="91"/>
+      <c r="H23" s="11"/>
+      <c r="I23" s="11">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="J23" s="11">
         <f t="shared" si="5"/>
-        <v>8.69</v>
-      </c>
-      <c r="I23" s="11">
+        <v>0</v>
+      </c>
+      <c r="K23" s="11">
         <f t="shared" si="6"/>
-        <v>8</v>
-      </c>
-      <c r="J23" s="11">
+        <v>0</v>
+      </c>
+      <c r="L23" s="12">
         <f t="shared" si="7"/>
         <v>0</v>
-      </c>
-      <c r="K23" s="11">
-        <f t="shared" si="8"/>
-        <v>0.69</v>
-      </c>
-      <c r="L23" s="12">
-        <f t="shared" si="9"/>
-        <v>8.69</v>
       </c>
     </row>
     <row r="24" spans="1:12">
       <c r="A24" s="63"/>
-      <c r="B24" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="C24" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="D24" s="62">
-        <f>CEILING(D23*0.3,1)</f>
-        <v>1</v>
-      </c>
+      <c r="B24" s="13"/>
+      <c r="C24" s="14"/>
+      <c r="D24" s="62"/>
       <c r="E24" s="86"/>
-      <c r="F24" s="88">
-        <v>3.2</v>
-      </c>
+      <c r="F24" s="88"/>
       <c r="G24" s="91"/>
-      <c r="H24" s="11">
+      <c r="H24" s="11"/>
+      <c r="I24" s="11">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="J24" s="11">
         <f t="shared" si="5"/>
-        <v>3.2</v>
-      </c>
-      <c r="I24" s="11">
+        <v>0</v>
+      </c>
+      <c r="K24" s="11">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="J24" s="11">
+      <c r="L24" s="12">
         <f t="shared" si="7"/>
-        <v>3.2</v>
-      </c>
-      <c r="K24" s="11">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="L24" s="12">
-        <f t="shared" si="9"/>
-        <v>3.2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:12">
       <c r="A25" s="63"/>
-      <c r="B25" s="13" t="s">
-        <v>70</v>
-      </c>
-      <c r="C25" s="14" t="s">
-        <v>71</v>
-      </c>
-      <c r="D25" s="62">
-        <f>ROUND(D23*1.2*1.5,2)</f>
-        <v>1.8</v>
-      </c>
+      <c r="B25" s="13"/>
+      <c r="C25" s="14"/>
+      <c r="D25" s="62"/>
       <c r="E25" s="86"/>
-      <c r="F25" s="88">
-        <v>0.55000000000000004</v>
-      </c>
+      <c r="F25" s="88"/>
       <c r="G25" s="91"/>
-      <c r="H25" s="11">
+      <c r="H25" s="11"/>
+      <c r="I25" s="11">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="J25" s="11">
         <f t="shared" si="5"/>
-        <v>0.55000000000000004</v>
-      </c>
-      <c r="I25" s="11">
+        <v>0</v>
+      </c>
+      <c r="K25" s="11">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="J25" s="11">
+      <c r="L25" s="12">
         <f t="shared" si="7"/>
-        <v>0.99</v>
-      </c>
-      <c r="K25" s="11">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="L25" s="12">
-        <f t="shared" si="9"/>
-        <v>0.99</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:12">
       <c r="A26" s="63"/>
-      <c r="B26" s="13" t="s">
-        <v>72</v>
-      </c>
-      <c r="C26" s="14" t="s">
-        <v>71</v>
-      </c>
-      <c r="D26" s="62">
-        <f>ROUND(D23*1.2,2)</f>
-        <v>1.2</v>
-      </c>
+      <c r="B26" s="13"/>
+      <c r="C26" s="14"/>
+      <c r="D26" s="62"/>
       <c r="E26" s="86"/>
-      <c r="F26" s="88">
-        <v>0.8</v>
-      </c>
+      <c r="F26" s="88"/>
       <c r="G26" s="91"/>
-      <c r="H26" s="11">
+      <c r="H26" s="11"/>
+      <c r="I26" s="11">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="J26" s="11">
         <f t="shared" si="5"/>
-        <v>0.8</v>
-      </c>
-      <c r="I26" s="11">
+        <v>0</v>
+      </c>
+      <c r="K26" s="11">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="J26" s="11">
+      <c r="L26" s="12">
         <f t="shared" si="7"/>
-        <v>0.96</v>
-      </c>
-      <c r="K26" s="11">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="L26" s="12">
-        <f t="shared" si="9"/>
-        <v>0.96</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:12">
       <c r="A27" s="63"/>
-      <c r="B27" s="13" t="s">
-        <v>73</v>
-      </c>
-      <c r="C27" s="14" t="s">
-        <v>74</v>
-      </c>
-      <c r="D27" s="12">
-        <f>ROUND(D23/45,2)</f>
-        <v>0.02</v>
-      </c>
+      <c r="B27" s="13"/>
+      <c r="C27" s="14"/>
+      <c r="D27" s="12"/>
       <c r="E27" s="51"/>
-      <c r="F27" s="51">
-        <v>1.43</v>
-      </c>
+      <c r="F27" s="51"/>
       <c r="G27" s="12"/>
-      <c r="H27" s="11">
+      <c r="H27" s="11"/>
+      <c r="I27" s="11">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="J27" s="11">
         <f t="shared" si="5"/>
-        <v>1.43</v>
-      </c>
-      <c r="I27" s="11">
+        <v>0</v>
+      </c>
+      <c r="K27" s="11">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="J27" s="11">
+      <c r="L27" s="12">
         <f t="shared" si="7"/>
-        <v>0.03</v>
-      </c>
-      <c r="K27" s="11">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="L27" s="12">
-        <f t="shared" si="9"/>
-        <v>0.03</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:12">
       <c r="A28" s="63"/>
-      <c r="B28" s="13" t="s">
-        <v>75</v>
-      </c>
-      <c r="C28" s="14" t="s">
-        <v>71</v>
-      </c>
-      <c r="D28" s="62">
-        <f>CEILING(D23*0.4,5)</f>
-        <v>5</v>
-      </c>
+      <c r="B28" s="13"/>
+      <c r="C28" s="14"/>
+      <c r="D28" s="62"/>
       <c r="E28" s="51"/>
-      <c r="F28" s="51">
-        <v>2.5</v>
-      </c>
+      <c r="F28" s="51"/>
       <c r="G28" s="12"/>
-      <c r="H28" s="11">
+      <c r="H28" s="11"/>
+      <c r="I28" s="11">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="J28" s="11">
         <f t="shared" si="5"/>
-        <v>2.5</v>
-      </c>
-      <c r="I28" s="11">
+        <v>0</v>
+      </c>
+      <c r="K28" s="11">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="J28" s="11">
+      <c r="L28" s="12">
         <f t="shared" si="7"/>
-        <v>12.5</v>
-      </c>
-      <c r="K28" s="11">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="L28" s="12">
-        <f t="shared" si="9"/>
-        <v>12.5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:12">
       <c r="A29" s="63"/>
-      <c r="B29" s="104" t="s">
-        <v>76</v>
-      </c>
-      <c r="C29" s="105" t="s">
-        <v>5</v>
-      </c>
-      <c r="D29" s="106">
-        <f>ROUND(D23*0.25,2)</f>
-        <v>0.25</v>
-      </c>
+      <c r="B29" s="104"/>
+      <c r="C29" s="105"/>
+      <c r="D29" s="106"/>
       <c r="E29" s="86"/>
-      <c r="F29" s="88">
-        <v>0.73</v>
-      </c>
+      <c r="F29" s="88"/>
       <c r="G29" s="91"/>
-      <c r="H29" s="11">
+      <c r="H29" s="11"/>
+      <c r="I29" s="11">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="J29" s="11">
         <f t="shared" si="5"/>
-        <v>0.73</v>
-      </c>
-      <c r="I29" s="11">
+        <v>0</v>
+      </c>
+      <c r="K29" s="11">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="J29" s="11">
+      <c r="L29" s="12">
         <f t="shared" si="7"/>
-        <v>0.18</v>
-      </c>
-      <c r="K29" s="11">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="L29" s="12">
-        <f t="shared" si="9"/>
-        <v>0.18</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:12">
       <c r="A30" s="63"/>
-      <c r="B30" s="16" t="s">
-        <v>77</v>
-      </c>
-      <c r="C30" s="42" t="s">
-        <v>11</v>
-      </c>
-      <c r="D30" s="62">
-        <v>19.8</v>
-      </c>
-      <c r="E30" s="12">
-        <v>7.5</v>
-      </c>
+      <c r="B30" s="16"/>
+      <c r="C30" s="42"/>
+      <c r="D30" s="62"/>
+      <c r="E30" s="12"/>
       <c r="F30" s="87"/>
-      <c r="G30" s="91">
-        <v>0.48</v>
-      </c>
-      <c r="H30" s="11">
+      <c r="G30" s="91"/>
+      <c r="H30" s="11"/>
+      <c r="I30" s="11">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="J30" s="11">
         <f t="shared" si="5"/>
-        <v>7.98</v>
-      </c>
-      <c r="I30" s="11">
+        <v>0</v>
+      </c>
+      <c r="K30" s="11">
         <f t="shared" si="6"/>
-        <v>148.5</v>
-      </c>
-      <c r="J30" s="11">
+        <v>0</v>
+      </c>
+      <c r="L30" s="12">
         <f t="shared" si="7"/>
         <v>0</v>
-      </c>
-      <c r="K30" s="11">
-        <f t="shared" si="8"/>
-        <v>9.5</v>
-      </c>
-      <c r="L30" s="12">
-        <f t="shared" si="9"/>
-        <v>158</v>
       </c>
     </row>
     <row r="31" spans="1:12">
       <c r="A31" s="63"/>
-      <c r="B31" s="41" t="s">
-        <v>78</v>
-      </c>
-      <c r="C31" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="D31" s="62">
-        <f>CEILING(D30*0.15,1)</f>
-        <v>3</v>
-      </c>
+      <c r="B31" s="41"/>
+      <c r="C31" s="14"/>
+      <c r="D31" s="62"/>
       <c r="E31" s="86"/>
-      <c r="F31" s="92">
-        <v>4.2</v>
-      </c>
+      <c r="F31" s="92"/>
       <c r="G31" s="91"/>
-      <c r="H31" s="11">
+      <c r="H31" s="11"/>
+      <c r="I31" s="11">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="J31" s="11">
         <f t="shared" si="5"/>
-        <v>4.2</v>
-      </c>
-      <c r="I31" s="11">
+        <v>0</v>
+      </c>
+      <c r="K31" s="11">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="J31" s="11">
+      <c r="L31" s="12">
         <f t="shared" si="7"/>
-        <v>12.6</v>
-      </c>
-      <c r="K31" s="11">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="L31" s="12">
-        <f t="shared" si="9"/>
-        <v>12.6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:12">
       <c r="A32" s="63"/>
-      <c r="B32" s="41" t="s">
-        <v>79</v>
-      </c>
-      <c r="C32" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="D32" s="62">
-        <f>CEILING(D30*0.3,1)</f>
-        <v>6</v>
-      </c>
+      <c r="B32" s="41"/>
+      <c r="C32" s="14"/>
+      <c r="D32" s="62"/>
       <c r="E32" s="86"/>
-      <c r="F32" s="92">
-        <v>5.82</v>
-      </c>
+      <c r="F32" s="92"/>
       <c r="G32" s="91"/>
-      <c r="H32" s="11">
+      <c r="H32" s="11"/>
+      <c r="I32" s="11">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="J32" s="11">
         <f t="shared" si="5"/>
-        <v>5.82</v>
-      </c>
-      <c r="I32" s="11">
+        <v>0</v>
+      </c>
+      <c r="K32" s="11">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="J32" s="11">
+      <c r="L32" s="12">
         <f t="shared" si="7"/>
-        <v>34.92</v>
-      </c>
-      <c r="K32" s="11">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="L32" s="12">
-        <f t="shared" si="9"/>
-        <v>34.92</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:13">
       <c r="A33" s="63"/>
-      <c r="B33" s="96" t="s">
-        <v>50</v>
-      </c>
-      <c r="C33" s="42" t="s">
-        <v>11</v>
-      </c>
-      <c r="D33" s="97">
-        <v>46</v>
-      </c>
-      <c r="E33" s="90">
-        <v>1.6</v>
-      </c>
+      <c r="B33" s="96"/>
+      <c r="C33" s="42"/>
+      <c r="D33" s="97"/>
+      <c r="E33" s="90"/>
       <c r="F33" s="90"/>
-      <c r="G33" s="91">
-        <v>0.33</v>
-      </c>
-      <c r="H33" s="12">
-        <f>ROUND(SUM(E33:G33),2)</f>
-        <v>1.93</v>
-      </c>
+      <c r="G33" s="91"/>
+      <c r="H33" s="12"/>
       <c r="I33" s="12">
-        <f t="shared" ref="I33:I37" si="10">ROUND(E33*D33,2)</f>
-        <v>73.599999999999994</v>
+        <f t="shared" ref="I33:I37" si="8">ROUND(E33*D33,2)</f>
+        <v>0</v>
       </c>
       <c r="J33" s="12">
-        <f t="shared" ref="J33:J37" si="11">ROUND(D33*F33,2)</f>
+        <f t="shared" ref="J33:J37" si="9">ROUND(D33*F33,2)</f>
         <v>0</v>
       </c>
       <c r="K33" s="12">
-        <f t="shared" ref="K33:K37" si="12">ROUND(D33*G33,2)</f>
-        <v>15.18</v>
+        <f t="shared" ref="K33:K37" si="10">ROUND(D33*G33,2)</f>
+        <v>0</v>
       </c>
       <c r="L33" s="12">
         <f>ROUND(SUM(I33:K33),2)</f>
-        <v>88.78</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:13">
       <c r="A34" s="63"/>
-      <c r="B34" s="16" t="s">
-        <v>51</v>
-      </c>
-      <c r="C34" s="42" t="s">
-        <v>11</v>
-      </c>
-      <c r="D34" s="62">
-        <f>D33</f>
-        <v>46</v>
-      </c>
-      <c r="E34" s="90">
-        <v>6.5</v>
-      </c>
+      <c r="B34" s="16"/>
+      <c r="C34" s="42"/>
+      <c r="D34" s="62"/>
+      <c r="E34" s="90"/>
       <c r="F34" s="51"/>
-      <c r="G34" s="91">
-        <v>0.24</v>
-      </c>
-      <c r="H34" s="12">
-        <f t="shared" ref="H34:H37" si="13">ROUND(SUM(E34:G34),2)</f>
-        <v>6.74</v>
-      </c>
+      <c r="G34" s="91"/>
+      <c r="H34" s="12"/>
       <c r="I34" s="12">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="J34" s="12">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="K34" s="12">
         <f t="shared" si="10"/>
-        <v>299</v>
-      </c>
-      <c r="J34" s="12">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="K34" s="12">
-        <f t="shared" si="12"/>
-        <v>11.04</v>
+        <v>0</v>
       </c>
       <c r="L34" s="12">
-        <f t="shared" ref="L34:L37" si="14">ROUND(SUM(I34:K34),2)</f>
-        <v>310.04000000000002</v>
+        <f t="shared" ref="L34:L37" si="11">ROUND(SUM(I34:K34),2)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:13">
       <c r="A35" s="63"/>
-      <c r="B35" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="C35" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="D35" s="62">
-        <f>ROUND(D34*0.15,2)</f>
-        <v>6.9</v>
-      </c>
+      <c r="B35" s="13"/>
+      <c r="C35" s="14"/>
+      <c r="D35" s="62"/>
       <c r="E35" s="86"/>
-      <c r="F35" s="88">
-        <v>3.2</v>
-      </c>
+      <c r="F35" s="88"/>
       <c r="G35" s="91"/>
-      <c r="H35" s="12">
-        <f t="shared" si="13"/>
-        <v>3.2</v>
-      </c>
+      <c r="H35" s="12"/>
       <c r="I35" s="12">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="J35" s="12">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="K35" s="12">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="J35" s="12">
+      <c r="L35" s="12">
         <f t="shared" si="11"/>
-        <v>22.08</v>
-      </c>
-      <c r="K35" s="12">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="L35" s="12">
-        <f t="shared" si="14"/>
-        <v>22.08</v>
+        <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:13">
       <c r="A36" s="63"/>
-      <c r="B36" s="41" t="s">
-        <v>52</v>
-      </c>
-      <c r="C36" s="42" t="s">
-        <v>11</v>
-      </c>
-      <c r="D36" s="98">
-        <f>CEILING(D34*1.4,5)</f>
-        <v>65</v>
-      </c>
+      <c r="B36" s="41"/>
+      <c r="C36" s="42"/>
+      <c r="D36" s="98"/>
       <c r="E36" s="86"/>
-      <c r="F36" s="92">
-        <v>2.75</v>
-      </c>
+      <c r="F36" s="92"/>
       <c r="G36" s="91"/>
-      <c r="H36" s="12">
-        <f t="shared" si="13"/>
-        <v>2.75</v>
-      </c>
+      <c r="H36" s="12"/>
       <c r="I36" s="12">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="J36" s="12">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="K36" s="12">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="J36" s="12">
+      <c r="L36" s="12">
         <f t="shared" si="11"/>
-        <v>178.75</v>
-      </c>
-      <c r="K36" s="12">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="L36" s="12">
-        <f t="shared" si="14"/>
-        <v>178.75</v>
+        <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:13">
       <c r="A37" s="63"/>
-      <c r="B37" s="41" t="s">
-        <v>53</v>
-      </c>
-      <c r="C37" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="D37" s="62">
-        <f>ROUND(D34*0.4,2)</f>
-        <v>18.399999999999999</v>
-      </c>
+      <c r="B37" s="41"/>
+      <c r="C37" s="14"/>
+      <c r="D37" s="62"/>
       <c r="E37" s="86"/>
-      <c r="F37" s="88">
-        <v>2.5099999999999998</v>
-      </c>
+      <c r="F37" s="88"/>
       <c r="G37" s="91"/>
-      <c r="H37" s="12">
-        <f t="shared" si="13"/>
-        <v>2.5099999999999998</v>
-      </c>
+      <c r="H37" s="12"/>
       <c r="I37" s="12">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="J37" s="12">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="K37" s="12">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="J37" s="12">
+      <c r="L37" s="12">
         <f t="shared" si="11"/>
-        <v>46.18</v>
-      </c>
-      <c r="K37" s="12">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="L37" s="12">
-        <f t="shared" si="14"/>
-        <v>46.18</v>
+        <v>0</v>
       </c>
     </row>
     <row r="38" spans="1:13">
       <c r="A38" s="63"/>
-      <c r="B38" s="96" t="s">
-        <v>54</v>
-      </c>
-      <c r="C38" s="42" t="s">
-        <v>11</v>
-      </c>
-      <c r="D38" s="15">
-        <v>19.8</v>
-      </c>
-      <c r="E38" s="12">
-        <v>2.5</v>
-      </c>
+      <c r="B38" s="96"/>
+      <c r="C38" s="42"/>
+      <c r="D38" s="15"/>
+      <c r="E38" s="12"/>
       <c r="F38" s="88"/>
-      <c r="G38" s="90">
-        <v>0.45</v>
-      </c>
-      <c r="H38" s="11">
-        <f t="shared" si="3"/>
-        <v>2.95</v>
-      </c>
+      <c r="G38" s="90"/>
+      <c r="H38" s="11"/>
       <c r="I38" s="11">
         <f>ROUND(E38*D38,2)</f>
-        <v>49.5</v>
+        <v>0</v>
       </c>
       <c r="J38" s="11">
         <f>ROUND(D38*F38,2)</f>
@@ -5432,291 +4999,199 @@
       </c>
       <c r="K38" s="11">
         <f>ROUND(D38*G38,2)</f>
-        <v>8.91</v>
+        <v>0</v>
       </c>
       <c r="L38" s="11">
-        <f t="shared" ref="L38:L40" si="15">ROUND(SUM(I38:K38),2)</f>
-        <v>58.41</v>
+        <f t="shared" ref="L38:L40" si="12">ROUND(SUM(I38:K38),2)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="39" spans="1:13">
       <c r="A39" s="63"/>
-      <c r="B39" s="99" t="s">
-        <v>55</v>
-      </c>
-      <c r="C39" s="42" t="s">
-        <v>11</v>
-      </c>
-      <c r="D39" s="62">
-        <f>D38</f>
-        <v>19.8</v>
-      </c>
-      <c r="E39" s="90">
-        <v>1.32</v>
-      </c>
+      <c r="B39" s="99"/>
+      <c r="C39" s="42"/>
+      <c r="D39" s="62"/>
+      <c r="E39" s="90"/>
       <c r="F39" s="90"/>
-      <c r="G39" s="12">
-        <f>ROUND(E39*10%,2)</f>
-        <v>0.13</v>
-      </c>
-      <c r="H39" s="11">
-        <f t="shared" si="3"/>
-        <v>1.45</v>
-      </c>
+      <c r="G39" s="12"/>
+      <c r="H39" s="11"/>
       <c r="I39" s="12">
-        <f t="shared" ref="I39:I45" si="16">ROUND(E39*D39,2)</f>
-        <v>26.14</v>
+        <f t="shared" ref="I39:I45" si="13">ROUND(E39*D39,2)</f>
+        <v>0</v>
       </c>
       <c r="J39" s="12">
-        <f t="shared" ref="J39:J45" si="17">ROUND(D39*F39,2)</f>
+        <f t="shared" ref="J39:J45" si="14">ROUND(D39*F39,2)</f>
         <v>0</v>
       </c>
       <c r="K39" s="12">
-        <f t="shared" ref="K39:K45" si="18">ROUND(D39*G39,2)</f>
-        <v>2.57</v>
+        <f t="shared" ref="K39:K45" si="15">ROUND(D39*G39,2)</f>
+        <v>0</v>
       </c>
       <c r="L39" s="11">
-        <f t="shared" si="15"/>
-        <v>28.71</v>
+        <f t="shared" si="12"/>
+        <v>0</v>
       </c>
     </row>
     <row r="40" spans="1:13">
       <c r="A40" s="63"/>
-      <c r="B40" s="100" t="s">
-        <v>56</v>
-      </c>
-      <c r="C40" s="42" t="s">
-        <v>11</v>
-      </c>
-      <c r="D40" s="62">
-        <f>ROUND(D39*1.1,2)</f>
-        <v>21.78</v>
-      </c>
+      <c r="B40" s="100"/>
+      <c r="C40" s="42"/>
+      <c r="D40" s="62"/>
       <c r="E40" s="12"/>
-      <c r="F40" s="88">
-        <v>1.76</v>
-      </c>
+      <c r="F40" s="88"/>
       <c r="G40" s="12"/>
-      <c r="H40" s="11">
-        <f t="shared" si="3"/>
-        <v>1.76</v>
-      </c>
+      <c r="H40" s="11"/>
       <c r="I40" s="12">
-        <f t="shared" si="16"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="J40" s="12">
-        <f t="shared" si="17"/>
-        <v>38.33</v>
+        <f t="shared" si="14"/>
+        <v>0</v>
       </c>
       <c r="K40" s="12">
-        <f t="shared" si="18"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="L40" s="11">
-        <f t="shared" si="15"/>
-        <v>38.33</v>
+        <f t="shared" si="12"/>
+        <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:13">
       <c r="A41" s="63"/>
-      <c r="B41" s="16" t="s">
-        <v>57</v>
-      </c>
-      <c r="C41" s="56" t="s">
-        <v>11</v>
-      </c>
-      <c r="D41" s="12">
-        <f>D39</f>
-        <v>19.8</v>
-      </c>
-      <c r="E41" s="12">
-        <v>7</v>
-      </c>
+      <c r="B41" s="16"/>
+      <c r="C41" s="56"/>
+      <c r="D41" s="12"/>
+      <c r="E41" s="12"/>
       <c r="F41" s="12"/>
-      <c r="G41" s="12">
-        <v>0.21</v>
-      </c>
-      <c r="H41" s="11">
-        <f t="shared" si="3"/>
-        <v>7.21</v>
-      </c>
+      <c r="G41" s="12"/>
+      <c r="H41" s="11"/>
       <c r="I41" s="11">
-        <f t="shared" si="16"/>
-        <v>138.6</v>
+        <f t="shared" si="13"/>
+        <v>0</v>
       </c>
       <c r="J41" s="11">
-        <f t="shared" si="17"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="K41" s="11">
-        <f t="shared" si="18"/>
-        <v>4.16</v>
+        <f t="shared" si="15"/>
+        <v>0</v>
       </c>
       <c r="L41" s="11">
-        <f t="shared" ref="L41:L45" si="19">ROUND(SUM(I41:K41),2)</f>
-        <v>142.76</v>
+        <f t="shared" ref="L41:L45" si="16">ROUND(SUM(I41:K41),2)</f>
+        <v>0</v>
       </c>
       <c r="M41" s="94"/>
     </row>
     <row r="42" spans="1:13">
       <c r="A42" s="63"/>
-      <c r="B42" s="101" t="s">
-        <v>58</v>
-      </c>
-      <c r="C42" s="56" t="s">
-        <v>11</v>
-      </c>
-      <c r="D42" s="12">
-        <f>ROUND(D41*1.1,2)</f>
-        <v>21.78</v>
-      </c>
+      <c r="B42" s="101"/>
+      <c r="C42" s="56"/>
+      <c r="D42" s="12"/>
       <c r="E42" s="12"/>
-      <c r="F42" s="12">
-        <v>11.4</v>
-      </c>
+      <c r="F42" s="12"/>
       <c r="G42" s="12"/>
-      <c r="H42" s="11">
-        <f t="shared" si="3"/>
-        <v>11.4</v>
-      </c>
+      <c r="H42" s="11"/>
       <c r="I42" s="11">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="J42" s="11">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="K42" s="11">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="L42" s="11">
         <f t="shared" si="16"/>
         <v>0</v>
-      </c>
-      <c r="J42" s="11">
-        <f t="shared" si="17"/>
-        <v>248.29</v>
-      </c>
-      <c r="K42" s="11">
-        <f t="shared" si="18"/>
-        <v>0</v>
-      </c>
-      <c r="L42" s="11">
-        <f t="shared" si="19"/>
-        <v>248.29</v>
       </c>
     </row>
     <row r="43" spans="1:13">
       <c r="A43" s="63"/>
-      <c r="B43" s="16" t="s">
-        <v>59</v>
-      </c>
-      <c r="C43" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="D43" s="12">
-        <v>16</v>
-      </c>
-      <c r="E43" s="12">
-        <v>3</v>
-      </c>
+      <c r="B43" s="16"/>
+      <c r="C43" s="14"/>
+      <c r="D43" s="12"/>
+      <c r="E43" s="12"/>
       <c r="F43" s="12"/>
-      <c r="G43" s="12">
-        <v>0.21</v>
-      </c>
-      <c r="H43" s="11">
-        <f t="shared" si="3"/>
-        <v>3.21</v>
-      </c>
+      <c r="G43" s="12"/>
+      <c r="H43" s="11"/>
       <c r="I43" s="12">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="J43" s="12">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="K43" s="12">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="L43" s="11">
         <f t="shared" si="16"/>
-        <v>48</v>
-      </c>
-      <c r="J43" s="12">
-        <f t="shared" si="17"/>
-        <v>0</v>
-      </c>
-      <c r="K43" s="12">
-        <f t="shared" si="18"/>
-        <v>3.36</v>
-      </c>
-      <c r="L43" s="11">
-        <f t="shared" si="19"/>
-        <v>51.36</v>
+        <v>0</v>
       </c>
     </row>
     <row r="44" spans="1:13">
       <c r="A44" s="63"/>
-      <c r="B44" s="13" t="s">
-        <v>60</v>
-      </c>
-      <c r="C44" s="14" t="s">
-        <v>61</v>
-      </c>
-      <c r="D44" s="62">
-        <f>ROUND(D43/0.4*1.1/100,2)</f>
-        <v>0.44</v>
-      </c>
+      <c r="B44" s="13"/>
+      <c r="C44" s="14"/>
+      <c r="D44" s="62"/>
       <c r="E44" s="86"/>
-      <c r="F44" s="87">
-        <v>19.5</v>
-      </c>
+      <c r="F44" s="87"/>
       <c r="G44" s="12"/>
-      <c r="H44" s="11">
-        <f t="shared" si="3"/>
-        <v>19.5</v>
-      </c>
+      <c r="H44" s="11"/>
       <c r="I44" s="11">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="J44" s="11">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="K44" s="11">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="L44" s="11">
         <f t="shared" si="16"/>
         <v>0</v>
-      </c>
-      <c r="J44" s="11">
-        <f t="shared" si="17"/>
-        <v>8.58</v>
-      </c>
-      <c r="K44" s="11">
-        <f t="shared" si="18"/>
-        <v>0</v>
-      </c>
-      <c r="L44" s="11">
-        <f t="shared" si="19"/>
-        <v>8.58</v>
       </c>
     </row>
     <row r="45" spans="1:13">
       <c r="A45" s="63"/>
-      <c r="B45" s="101" t="s">
-        <v>62</v>
-      </c>
-      <c r="C45" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="D45" s="12">
-        <f>CEILING(D43*1.1,2.4)</f>
-        <v>19.2</v>
-      </c>
+      <c r="B45" s="101"/>
+      <c r="C45" s="14"/>
+      <c r="D45" s="12"/>
       <c r="E45" s="12"/>
-      <c r="F45" s="12">
-        <v>2.0499999999999998</v>
-      </c>
+      <c r="F45" s="12"/>
       <c r="G45" s="12"/>
-      <c r="H45" s="11">
-        <f t="shared" si="3"/>
-        <v>2.0499999999999998</v>
-      </c>
+      <c r="H45" s="11"/>
       <c r="I45" s="11">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="J45" s="11">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="K45" s="11">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="L45" s="11">
         <f t="shared" si="16"/>
         <v>0</v>
-      </c>
-      <c r="J45" s="11">
-        <f t="shared" si="17"/>
-        <v>39.36</v>
-      </c>
-      <c r="K45" s="11">
-        <f t="shared" si="18"/>
-        <v>0</v>
-      </c>
-      <c r="L45" s="11">
-        <f t="shared" si="19"/>
-        <v>39.36</v>
       </c>
     </row>
     <row r="46" spans="1:13">
       <c r="A46" s="79"/>
-      <c r="B46" s="58" t="s">
-        <v>80</v>
-      </c>
+      <c r="B46" s="58"/>
       <c r="C46" s="61"/>
       <c r="D46" s="59"/>
       <c r="E46" s="59"/>
@@ -5730,171 +5205,111 @@
     </row>
     <row r="47" spans="1:13">
       <c r="A47" s="63"/>
-      <c r="B47" s="107" t="s">
-        <v>81</v>
-      </c>
-      <c r="C47" s="56" t="s">
-        <v>11</v>
-      </c>
-      <c r="D47" s="56">
-        <v>10</v>
-      </c>
-      <c r="E47" s="54">
-        <v>2.5299999999999998</v>
-      </c>
+      <c r="B47" s="107"/>
+      <c r="C47" s="56"/>
+      <c r="D47" s="56"/>
+      <c r="E47" s="54"/>
       <c r="F47" s="50"/>
-      <c r="G47" s="108">
-        <f t="shared" ref="G47" si="20">ROUND(E47*10%,2)</f>
-        <v>0.25</v>
-      </c>
-      <c r="H47" s="11">
-        <f t="shared" ref="H47" si="21">ROUND(SUM(E47:G47),2)</f>
-        <v>2.78</v>
-      </c>
+      <c r="G47" s="108"/>
+      <c r="H47" s="11"/>
       <c r="I47" s="55">
-        <f t="shared" ref="I47:I48" si="22">ROUND(E47*D47,2)</f>
-        <v>25.3</v>
+        <f t="shared" ref="I47:I48" si="17">ROUND(E47*D47,2)</f>
+        <v>0</v>
       </c>
       <c r="J47" s="55">
-        <f t="shared" ref="J47" si="23">ROUND(F47*D47,2)</f>
+        <f t="shared" ref="J47" si="18">ROUND(F47*D47,2)</f>
         <v>0</v>
       </c>
       <c r="K47" s="55">
-        <f t="shared" ref="K47" si="24">ROUND(G47*D47,2)</f>
-        <v>2.5</v>
+        <f t="shared" ref="K47" si="19">ROUND(G47*D47,2)</f>
+        <v>0</v>
       </c>
       <c r="L47" s="55">
-        <f t="shared" ref="L47:L48" si="25">ROUND(SUM(I47:K47),2)</f>
-        <v>27.8</v>
+        <f t="shared" ref="L47:L48" si="20">ROUND(SUM(I47:K47),2)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="48" spans="1:13" s="110" customFormat="1">
       <c r="A48" s="63"/>
-      <c r="B48" s="109" t="s">
-        <v>82</v>
-      </c>
-      <c r="C48" s="14" t="s">
-        <v>83</v>
-      </c>
-      <c r="D48" s="11">
-        <v>1</v>
-      </c>
-      <c r="E48" s="12">
-        <v>1000</v>
-      </c>
-      <c r="F48" s="12">
-        <v>700</v>
-      </c>
-      <c r="G48" s="108">
-        <v>300</v>
-      </c>
-      <c r="H48" s="11">
-        <f>ROUND(SUM(E48:G48),2)</f>
-        <v>2000</v>
-      </c>
+      <c r="B48" s="109"/>
+      <c r="C48" s="14"/>
+      <c r="D48" s="11"/>
+      <c r="E48" s="12"/>
+      <c r="F48" s="12"/>
+      <c r="G48" s="108"/>
+      <c r="H48" s="11"/>
       <c r="I48" s="11">
-        <f t="shared" si="22"/>
-        <v>1000</v>
+        <f t="shared" si="17"/>
+        <v>0</v>
       </c>
       <c r="J48" s="11">
-        <f t="shared" ref="J48" si="26">ROUND(D48*F48,2)</f>
-        <v>700</v>
+        <f t="shared" ref="J48" si="21">ROUND(D48*F48,2)</f>
+        <v>0</v>
       </c>
       <c r="K48" s="11">
-        <f t="shared" ref="K48" si="27">ROUND(D48*G48,2)</f>
-        <v>300</v>
+        <f t="shared" ref="K48" si="22">ROUND(D48*G48,2)</f>
+        <v>0</v>
       </c>
       <c r="L48" s="11">
-        <f t="shared" si="25"/>
-        <v>2000</v>
+        <f t="shared" si="20"/>
+        <v>0</v>
       </c>
     </row>
     <row r="49" spans="1:12">
       <c r="A49" s="63"/>
-      <c r="B49" s="107" t="s">
-        <v>84</v>
-      </c>
-      <c r="C49" s="56" t="s">
-        <v>11</v>
-      </c>
-      <c r="D49" s="56">
-        <v>10</v>
-      </c>
-      <c r="E49" s="54">
-        <v>8.8000000000000007</v>
-      </c>
-      <c r="F49" s="50">
-        <v>0.08</v>
-      </c>
-      <c r="G49" s="108">
-        <f t="shared" ref="G49" si="28">ROUND(E49*10%,2)</f>
-        <v>0.88</v>
-      </c>
-      <c r="H49" s="11">
-        <f t="shared" ref="H49" si="29">ROUND(SUM(E49:G49),2)</f>
-        <v>9.76</v>
-      </c>
+      <c r="B49" s="107"/>
+      <c r="C49" s="56"/>
+      <c r="D49" s="56"/>
+      <c r="E49" s="54"/>
+      <c r="F49" s="50"/>
+      <c r="G49" s="108"/>
+      <c r="H49" s="11"/>
       <c r="I49" s="55">
-        <f t="shared" ref="I49:I50" si="30">ROUND(E49*D49,2)</f>
-        <v>88</v>
+        <f t="shared" ref="I49:I50" si="23">ROUND(E49*D49,2)</f>
+        <v>0</v>
       </c>
       <c r="J49" s="55">
-        <f t="shared" ref="J49" si="31">ROUND(F49*D49,2)</f>
-        <v>0.8</v>
+        <f t="shared" ref="J49" si="24">ROUND(F49*D49,2)</f>
+        <v>0</v>
       </c>
       <c r="K49" s="55">
-        <f t="shared" ref="K49" si="32">ROUND(G49*D49,2)</f>
-        <v>8.8000000000000007</v>
+        <f t="shared" ref="K49" si="25">ROUND(G49*D49,2)</f>
+        <v>0</v>
       </c>
       <c r="L49" s="55">
-        <f t="shared" ref="L49:L50" si="33">ROUND(SUM(I49:K49),2)</f>
-        <v>97.6</v>
+        <f t="shared" ref="L49:L50" si="26">ROUND(SUM(I49:K49),2)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="50" spans="1:12">
       <c r="A50" s="82"/>
-      <c r="B50" s="16" t="s">
-        <v>85</v>
-      </c>
-      <c r="C50" s="95" t="s">
-        <v>86</v>
-      </c>
-      <c r="D50" s="12">
-        <v>2</v>
-      </c>
-      <c r="E50" s="50">
-        <v>17.600000000000001</v>
-      </c>
+      <c r="B50" s="16"/>
+      <c r="C50" s="95"/>
+      <c r="D50" s="12"/>
+      <c r="E50" s="50"/>
       <c r="F50" s="51"/>
-      <c r="G50" s="51">
-        <v>26.4</v>
-      </c>
-      <c r="H50" s="12">
-        <f t="shared" ref="H50" si="34">ROUND(SUM(E50:G50),2)</f>
-        <v>44</v>
-      </c>
+      <c r="G50" s="51"/>
+      <c r="H50" s="12"/>
       <c r="I50" s="12">
-        <f t="shared" si="30"/>
-        <v>35.200000000000003</v>
+        <f t="shared" si="23"/>
+        <v>0</v>
       </c>
       <c r="J50" s="12">
-        <f t="shared" ref="J50" si="35">ROUND(D50*F50,2)</f>
+        <f t="shared" ref="J50" si="27">ROUND(D50*F50,2)</f>
         <v>0</v>
       </c>
       <c r="K50" s="12">
-        <f t="shared" ref="K50" si="36">ROUND(D50*G50,2)</f>
-        <v>52.8</v>
+        <f t="shared" ref="K50" si="28">ROUND(D50*G50,2)</f>
+        <v>0</v>
       </c>
       <c r="L50" s="12">
-        <f t="shared" si="33"/>
-        <v>88</v>
+        <f t="shared" si="26"/>
+        <v>0</v>
       </c>
     </row>
     <row r="51" spans="1:12">
       <c r="A51" s="79"/>
-      <c r="B51" s="58" t="s">
-        <v>88</v>
-      </c>
+      <c r="B51" s="58"/>
       <c r="C51" s="61"/>
       <c r="D51" s="59"/>
       <c r="E51" s="59"/>
@@ -5907,285 +5322,185 @@
       <c r="L51" s="59"/>
     </row>
     <row r="52" spans="1:12">
-      <c r="A52" s="115"/>
-      <c r="B52" s="116" t="s">
-        <v>81</v>
-      </c>
-      <c r="C52" s="117" t="s">
-        <v>11</v>
-      </c>
-      <c r="D52" s="117">
-        <v>20</v>
-      </c>
-      <c r="E52" s="118">
-        <v>2.5299999999999998</v>
-      </c>
-      <c r="F52" s="119"/>
-      <c r="G52" s="120">
-        <f t="shared" ref="G52" si="37">ROUND(E52*10%,2)</f>
-        <v>0.25</v>
-      </c>
-      <c r="H52" s="121">
-        <f t="shared" ref="H52" si="38">ROUND(SUM(E52:G52),2)</f>
-        <v>2.78</v>
-      </c>
-      <c r="I52" s="122">
-        <f t="shared" ref="I52:I58" si="39">ROUND(E52*D52,2)</f>
-        <v>50.6</v>
-      </c>
-      <c r="J52" s="122">
-        <f t="shared" ref="J52" si="40">ROUND(F52*D52,2)</f>
-        <v>0</v>
-      </c>
-      <c r="K52" s="122">
-        <f t="shared" ref="K52" si="41">ROUND(G52*D52,2)</f>
-        <v>5</v>
-      </c>
-      <c r="L52" s="122">
-        <f t="shared" ref="L52:L54" si="42">ROUND(SUM(I52:K52),2)</f>
-        <v>55.6</v>
+      <c r="A52" s="111"/>
+      <c r="B52" s="112"/>
+      <c r="C52" s="113"/>
+      <c r="D52" s="113"/>
+      <c r="E52" s="114"/>
+      <c r="F52" s="115"/>
+      <c r="G52" s="116"/>
+      <c r="H52" s="117"/>
+      <c r="I52" s="118">
+        <f t="shared" ref="I52:I58" si="29">ROUND(E52*D52,2)</f>
+        <v>0</v>
+      </c>
+      <c r="J52" s="118">
+        <f t="shared" ref="J52" si="30">ROUND(F52*D52,2)</f>
+        <v>0</v>
+      </c>
+      <c r="K52" s="118">
+        <f t="shared" ref="K52" si="31">ROUND(G52*D52,2)</f>
+        <v>0</v>
+      </c>
+      <c r="L52" s="118">
+        <f t="shared" ref="L52:L54" si="32">ROUND(SUM(I52:K52),2)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="53" spans="1:12">
-      <c r="A53" s="115"/>
-      <c r="B53" s="116" t="s">
-        <v>87</v>
-      </c>
-      <c r="C53" s="117" t="s">
-        <v>11</v>
-      </c>
-      <c r="D53" s="117">
-        <f>D52</f>
-        <v>20</v>
-      </c>
-      <c r="E53" s="118">
-        <v>8.8000000000000007</v>
-      </c>
-      <c r="F53" s="119">
-        <v>21</v>
-      </c>
-      <c r="G53" s="120">
-        <f t="shared" ref="G53" si="43">ROUND(E53*10%,2)</f>
-        <v>0.88</v>
-      </c>
-      <c r="H53" s="121">
-        <f t="shared" ref="H53" si="44">ROUND(SUM(E53:G53),2)</f>
-        <v>30.68</v>
-      </c>
-      <c r="I53" s="122">
+      <c r="A53" s="111"/>
+      <c r="B53" s="112"/>
+      <c r="C53" s="113"/>
+      <c r="D53" s="113"/>
+      <c r="E53" s="114"/>
+      <c r="F53" s="115"/>
+      <c r="G53" s="116"/>
+      <c r="H53" s="117"/>
+      <c r="I53" s="118">
+        <f t="shared" si="29"/>
+        <v>0</v>
+      </c>
+      <c r="J53" s="118">
+        <f t="shared" ref="J53" si="33">ROUND(F53*D53,2)</f>
+        <v>0</v>
+      </c>
+      <c r="K53" s="118">
+        <f t="shared" ref="K53" si="34">ROUND(G53*D53,2)</f>
+        <v>0</v>
+      </c>
+      <c r="L53" s="118">
+        <f t="shared" si="32"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12">
+      <c r="A54" s="111"/>
+      <c r="B54" s="119"/>
+      <c r="C54" s="120"/>
+      <c r="D54" s="120"/>
+      <c r="E54" s="114"/>
+      <c r="F54" s="114"/>
+      <c r="G54" s="116"/>
+      <c r="H54" s="117"/>
+      <c r="I54" s="117">
+        <f t="shared" si="29"/>
+        <v>0</v>
+      </c>
+      <c r="J54" s="117">
+        <f t="shared" ref="J54" si="35">ROUND(D54*F54,2)</f>
+        <v>0</v>
+      </c>
+      <c r="K54" s="117">
+        <f t="shared" ref="K54" si="36">ROUND(D54*G54,2)</f>
+        <v>0</v>
+      </c>
+      <c r="L54" s="117">
+        <f t="shared" si="32"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12">
+      <c r="A55" s="111"/>
+      <c r="B55" s="121"/>
+      <c r="C55" s="122"/>
+      <c r="D55" s="117"/>
+      <c r="E55" s="117"/>
+      <c r="F55" s="117"/>
+      <c r="G55" s="116"/>
+      <c r="H55" s="117"/>
+      <c r="I55" s="117">
+        <f t="shared" si="29"/>
+        <v>0</v>
+      </c>
+      <c r="J55" s="117">
+        <f t="shared" ref="J55:J57" si="37">ROUND(F55*D55,2)</f>
+        <v>0</v>
+      </c>
+      <c r="K55" s="117">
+        <f t="shared" ref="K55:K57" si="38">ROUND(G55*D55,2)</f>
+        <v>0</v>
+      </c>
+      <c r="L55" s="117">
+        <f t="shared" ref="L55:L57" si="39">ROUND(I55+J55+K55,2)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12">
+      <c r="A56" s="111"/>
+      <c r="B56" s="112"/>
+      <c r="C56" s="113"/>
+      <c r="D56" s="113"/>
+      <c r="E56" s="114"/>
+      <c r="F56" s="115"/>
+      <c r="G56" s="116"/>
+      <c r="H56" s="117"/>
+      <c r="I56" s="118">
+        <f t="shared" si="29"/>
+        <v>0</v>
+      </c>
+      <c r="J56" s="118">
+        <f t="shared" si="37"/>
+        <v>0</v>
+      </c>
+      <c r="K56" s="118">
+        <f t="shared" si="38"/>
+        <v>0</v>
+      </c>
+      <c r="L56" s="118">
         <f t="shared" si="39"/>
-        <v>176</v>
-      </c>
-      <c r="J53" s="122">
-        <f t="shared" ref="J53" si="45">ROUND(F53*D53,2)</f>
-        <v>420</v>
-      </c>
-      <c r="K53" s="122">
-        <f t="shared" ref="K53" si="46">ROUND(G53*D53,2)</f>
-        <v>17.600000000000001</v>
-      </c>
-      <c r="L53" s="122">
-        <f t="shared" si="42"/>
-        <v>613.6</v>
-      </c>
-    </row>
-    <row r="54" spans="1:12">
-      <c r="A54" s="115"/>
-      <c r="B54" s="123" t="s">
-        <v>68</v>
-      </c>
-      <c r="C54" s="124" t="s">
-        <v>11</v>
-      </c>
-      <c r="D54" s="124">
-        <v>10</v>
-      </c>
-      <c r="E54" s="118">
-        <v>1.6</v>
-      </c>
-      <c r="F54" s="118"/>
-      <c r="G54" s="120">
-        <v>0.22</v>
-      </c>
-      <c r="H54" s="121">
-        <f t="shared" ref="H54" si="47">ROUND(SUM(E54:G54),2)</f>
-        <v>1.82</v>
-      </c>
-      <c r="I54" s="121">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12">
+      <c r="A57" s="111"/>
+      <c r="B57" s="123"/>
+      <c r="C57" s="113"/>
+      <c r="D57" s="117"/>
+      <c r="E57" s="115"/>
+      <c r="F57" s="115"/>
+      <c r="G57" s="115"/>
+      <c r="H57" s="117"/>
+      <c r="I57" s="117">
+        <f t="shared" si="29"/>
+        <v>0</v>
+      </c>
+      <c r="J57" s="117">
+        <f t="shared" si="37"/>
+        <v>0</v>
+      </c>
+      <c r="K57" s="117">
+        <f t="shared" si="38"/>
+        <v>0</v>
+      </c>
+      <c r="L57" s="117">
         <f t="shared" si="39"/>
-        <v>16</v>
-      </c>
-      <c r="J54" s="121">
-        <f t="shared" ref="J54" si="48">ROUND(D54*F54,2)</f>
-        <v>0</v>
-      </c>
-      <c r="K54" s="121">
-        <f t="shared" ref="K54" si="49">ROUND(D54*G54,2)</f>
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="L54" s="121">
-        <f t="shared" si="42"/>
-        <v>18.2</v>
-      </c>
-    </row>
-    <row r="55" spans="1:12">
-      <c r="A55" s="115"/>
-      <c r="B55" s="125" t="s">
-        <v>89</v>
-      </c>
-      <c r="C55" s="126" t="s">
-        <v>11</v>
-      </c>
-      <c r="D55" s="121">
-        <f>D54</f>
-        <v>10</v>
-      </c>
-      <c r="E55" s="121">
-        <v>2.15</v>
-      </c>
-      <c r="F55" s="121"/>
-      <c r="G55" s="120">
-        <v>0.11550000000000002</v>
-      </c>
-      <c r="H55" s="121">
-        <f t="shared" ref="H55:H57" si="50">ROUND(E55+F55+G55,2)</f>
-        <v>2.27</v>
-      </c>
-      <c r="I55" s="121">
-        <f t="shared" si="39"/>
-        <v>21.5</v>
-      </c>
-      <c r="J55" s="121">
-        <f t="shared" ref="J55:J57" si="51">ROUND(F55*D55,2)</f>
-        <v>0</v>
-      </c>
-      <c r="K55" s="121">
-        <f t="shared" ref="K55:K57" si="52">ROUND(G55*D55,2)</f>
-        <v>1.1599999999999999</v>
-      </c>
-      <c r="L55" s="121">
-        <f t="shared" ref="L55:L57" si="53">ROUND(I55+J55+K55,2)</f>
-        <v>22.66</v>
-      </c>
-    </row>
-    <row r="56" spans="1:12">
-      <c r="A56" s="115"/>
-      <c r="B56" s="116" t="s">
-        <v>90</v>
-      </c>
-      <c r="C56" s="117" t="s">
-        <v>11</v>
-      </c>
-      <c r="D56" s="117">
-        <f>CEILING(D55*1.1,3.12)</f>
-        <v>12.48</v>
-      </c>
-      <c r="E56" s="118"/>
-      <c r="F56" s="119">
-        <v>1.61</v>
-      </c>
-      <c r="G56" s="120">
-        <v>0</v>
-      </c>
-      <c r="H56" s="121">
-        <f t="shared" si="50"/>
-        <v>1.61</v>
-      </c>
-      <c r="I56" s="122">
-        <f t="shared" si="39"/>
-        <v>0</v>
-      </c>
-      <c r="J56" s="122">
-        <f t="shared" si="51"/>
-        <v>20.09</v>
-      </c>
-      <c r="K56" s="122">
-        <f t="shared" si="52"/>
-        <v>0</v>
-      </c>
-      <c r="L56" s="122">
-        <f t="shared" si="53"/>
-        <v>20.09</v>
-      </c>
-    </row>
-    <row r="57" spans="1:12">
-      <c r="A57" s="115"/>
-      <c r="B57" s="127" t="s">
-        <v>91</v>
-      </c>
-      <c r="C57" s="117" t="s">
-        <v>11</v>
-      </c>
-      <c r="D57" s="121">
-        <f>D55</f>
-        <v>10</v>
-      </c>
-      <c r="E57" s="119"/>
-      <c r="F57" s="119">
-        <v>0.64</v>
-      </c>
-      <c r="G57" s="119">
-        <v>0</v>
-      </c>
-      <c r="H57" s="121">
-        <f t="shared" si="50"/>
-        <v>0.64</v>
-      </c>
-      <c r="I57" s="121">
-        <f t="shared" si="39"/>
-        <v>0</v>
-      </c>
-      <c r="J57" s="121">
-        <f t="shared" si="51"/>
-        <v>6.4</v>
-      </c>
-      <c r="K57" s="121">
-        <f t="shared" si="52"/>
-        <v>0</v>
-      </c>
-      <c r="L57" s="121">
-        <f t="shared" si="53"/>
-        <v>6.4</v>
-      </c>
-    </row>
-    <row r="58" spans="1:12" ht="24">
-      <c r="A58" s="115"/>
-      <c r="B58" s="127" t="s">
-        <v>92</v>
-      </c>
-      <c r="C58" s="126" t="s">
-        <v>93</v>
-      </c>
-      <c r="D58" s="121">
-        <v>2</v>
-      </c>
-      <c r="E58" s="118">
-        <v>12.1</v>
-      </c>
-      <c r="F58" s="119"/>
-      <c r="G58" s="121">
-        <f t="shared" ref="G58" si="54">ROUND(E58*10%,2)</f>
-        <v>1.21</v>
-      </c>
-      <c r="H58" s="121">
-        <f t="shared" ref="H58" si="55">ROUND(SUM(E58:G58),2)</f>
-        <v>13.31</v>
-      </c>
-      <c r="I58" s="121">
-        <f t="shared" si="39"/>
-        <v>24.2</v>
-      </c>
-      <c r="J58" s="121">
-        <f t="shared" ref="J58" si="56">ROUND(D58*F58,2)</f>
-        <v>0</v>
-      </c>
-      <c r="K58" s="121">
-        <f t="shared" ref="K58" si="57">ROUND(D58*G58,2)</f>
-        <v>2.42</v>
-      </c>
-      <c r="L58" s="121">
-        <f t="shared" ref="L58" si="58">ROUND(SUM(I58:K58),2)</f>
-        <v>26.62</v>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12">
+      <c r="A58" s="111"/>
+      <c r="B58" s="123"/>
+      <c r="C58" s="122"/>
+      <c r="D58" s="117"/>
+      <c r="E58" s="114"/>
+      <c r="F58" s="115"/>
+      <c r="G58" s="117"/>
+      <c r="H58" s="117"/>
+      <c r="I58" s="117">
+        <f t="shared" si="29"/>
+        <v>0</v>
+      </c>
+      <c r="J58" s="117">
+        <f t="shared" ref="J58" si="40">ROUND(D58*F58,2)</f>
+        <v>0</v>
+      </c>
+      <c r="K58" s="117">
+        <f t="shared" ref="K58" si="41">ROUND(D58*G58,2)</f>
+        <v>0</v>
+      </c>
+      <c r="L58" s="117">
+        <f t="shared" ref="L58" si="42">ROUND(SUM(I58:K58),2)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="59" spans="1:12">
@@ -6204,30 +5519,16 @@
     </row>
     <row r="60" spans="1:12">
       <c r="A60" s="82"/>
-      <c r="B60" s="80" t="s">
-        <v>35</v>
-      </c>
-      <c r="C60" s="53" t="s">
-        <v>26</v>
-      </c>
-      <c r="D60" s="62">
-        <v>16</v>
-      </c>
-      <c r="E60" s="52">
-        <v>6.8</v>
-      </c>
+      <c r="B60" s="80"/>
+      <c r="C60" s="53"/>
+      <c r="D60" s="62"/>
+      <c r="E60" s="52"/>
       <c r="F60" s="51"/>
-      <c r="G60" s="51">
-        <f>ROUND(E60*10%,2)</f>
-        <v>0.68</v>
-      </c>
-      <c r="H60" s="12">
-        <f>ROUND(SUM(E60:G60),2)</f>
-        <v>7.48</v>
-      </c>
+      <c r="G60" s="51"/>
+      <c r="H60" s="12"/>
       <c r="I60" s="12">
         <f>ROUND(E60*D60,2)</f>
-        <v>108.8</v>
+        <v>0</v>
       </c>
       <c r="J60" s="12">
         <f>ROUND(D60*F60,2)</f>
@@ -6235,124 +5536,77 @@
       </c>
       <c r="K60" s="12">
         <f>ROUND(D60*G60,2)</f>
-        <v>10.88</v>
+        <v>0</v>
       </c>
       <c r="L60" s="12">
         <f>ROUND(SUM(I60:K60),2)</f>
-        <v>119.68</v>
+        <v>0</v>
       </c>
     </row>
     <row r="61" spans="1:12">
       <c r="A61" s="83"/>
-      <c r="B61" s="57" t="s">
-        <v>49</v>
-      </c>
-      <c r="C61" s="56" t="s">
-        <v>29</v>
-      </c>
-      <c r="D61" s="56">
-        <v>1</v>
-      </c>
-      <c r="E61" s="54">
-        <v>65</v>
-      </c>
-      <c r="F61" s="50">
-        <f>0.7*60</f>
-        <v>42</v>
-      </c>
-      <c r="G61" s="50">
-        <f>0.2*60</f>
-        <v>12</v>
-      </c>
-      <c r="H61" s="50">
-        <f t="shared" ref="H61:H62" si="59">ROUND(SUM(E61:G61),2)</f>
-        <v>119</v>
-      </c>
+      <c r="B61" s="57"/>
+      <c r="C61" s="56"/>
+      <c r="D61" s="56"/>
+      <c r="E61" s="54"/>
+      <c r="F61" s="50"/>
+      <c r="G61" s="50"/>
+      <c r="H61" s="50"/>
       <c r="I61" s="55">
-        <f t="shared" ref="I61:I62" si="60">ROUND(E61*D61,2)</f>
-        <v>65</v>
+        <f t="shared" ref="I61:I62" si="43">ROUND(E61*D61,2)</f>
+        <v>0</v>
       </c>
       <c r="J61" s="55">
-        <f t="shared" ref="J61:J62" si="61">ROUND(F61*D61,2)</f>
-        <v>42</v>
+        <f t="shared" ref="J61:J62" si="44">ROUND(F61*D61,2)</f>
+        <v>0</v>
       </c>
       <c r="K61" s="55">
-        <f t="shared" ref="K61:K62" si="62">ROUND(G61*D61,2)</f>
-        <v>12</v>
+        <f t="shared" ref="K61:K62" si="45">ROUND(G61*D61,2)</f>
+        <v>0</v>
       </c>
       <c r="L61" s="55">
-        <f t="shared" ref="L61:L62" si="63">ROUND(SUM(I61:K61),2)</f>
-        <v>119</v>
+        <f t="shared" ref="L61:L62" si="46">ROUND(SUM(I61:K61),2)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="62" spans="1:12">
       <c r="A62" s="83"/>
-      <c r="B62" s="57" t="s">
-        <v>47</v>
-      </c>
-      <c r="C62" s="56" t="s">
-        <v>29</v>
-      </c>
-      <c r="D62" s="56">
-        <v>1</v>
-      </c>
-      <c r="E62" s="54">
-        <v>141</v>
-      </c>
-      <c r="F62" s="50">
-        <f>0.42*60</f>
-        <v>25.2</v>
-      </c>
-      <c r="G62" s="50">
-        <f>ROUND(60*0.5,2)</f>
-        <v>30</v>
-      </c>
-      <c r="H62" s="50">
-        <f t="shared" si="59"/>
-        <v>196.2</v>
-      </c>
+      <c r="B62" s="57"/>
+      <c r="C62" s="56"/>
+      <c r="D62" s="56"/>
+      <c r="E62" s="54"/>
+      <c r="F62" s="50"/>
+      <c r="G62" s="50"/>
+      <c r="H62" s="50"/>
       <c r="I62" s="55">
-        <f t="shared" si="60"/>
-        <v>141</v>
+        <f t="shared" si="43"/>
+        <v>0</v>
       </c>
       <c r="J62" s="55">
-        <f t="shared" si="61"/>
-        <v>25.2</v>
+        <f t="shared" si="44"/>
+        <v>0</v>
       </c>
       <c r="K62" s="55">
-        <f t="shared" si="62"/>
-        <v>30</v>
+        <f t="shared" si="45"/>
+        <v>0</v>
       </c>
       <c r="L62" s="55">
-        <f t="shared" si="63"/>
-        <v>196.2</v>
+        <f t="shared" si="46"/>
+        <v>0</v>
       </c>
     </row>
     <row r="63" spans="1:12">
       <c r="A63" s="83"/>
-      <c r="B63" s="16" t="s">
-        <v>48</v>
-      </c>
-      <c r="C63" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="D63" s="15">
-        <v>1</v>
-      </c>
-      <c r="E63" s="86">
-        <v>22.93</v>
-      </c>
+      <c r="B63" s="16"/>
+      <c r="C63" s="14"/>
+      <c r="D63" s="15"/>
+      <c r="E63" s="86"/>
       <c r="F63" s="92"/>
-      <c r="G63" s="93">
-        <v>61.7</v>
-      </c>
-      <c r="H63" s="50">
-        <f t="shared" ref="H63" si="64">ROUND(SUM(E63:G63),2)</f>
-        <v>84.63</v>
-      </c>
+      <c r="G63" s="93"/>
+      <c r="H63" s="50"/>
       <c r="I63" s="11">
-        <f t="shared" ref="I63" si="65">ROUND(E63*D63,2)</f>
-        <v>22.93</v>
+        <f t="shared" ref="I63" si="47">ROUND(E63*D63,2)</f>
+        <v>0</v>
       </c>
       <c r="J63" s="11">
         <f>ROUND(D63*F63,2)</f>
@@ -6360,17 +5614,17 @@
       </c>
       <c r="K63" s="11">
         <f>ROUND(D63*G63,2)</f>
-        <v>61.7</v>
+        <v>0</v>
       </c>
       <c r="L63" s="11">
-        <f t="shared" ref="L63" si="66">ROUND(SUM(I63:K63),2)</f>
-        <v>84.63</v>
+        <f t="shared" ref="L63" si="48">ROUND(SUM(I63:K63),2)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="64" spans="1:12">
       <c r="A64" s="17"/>
       <c r="B64" s="18" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C64" s="77"/>
       <c r="D64" s="19"/>
@@ -6380,25 +5634,25 @@
       <c r="H64" s="19"/>
       <c r="I64" s="19">
         <f>SUM(I15:I63)</f>
-        <v>2883.3699999999994</v>
+        <v>0</v>
       </c>
       <c r="J64" s="19">
         <f>SUM(J15:J63)</f>
-        <v>2070.5699999999997</v>
+        <v>0</v>
       </c>
       <c r="K64" s="19">
         <f>SUM(K15:K63)</f>
-        <v>584.92000000000007</v>
+        <v>0</v>
       </c>
       <c r="L64" s="19">
         <f>SUM(L15:L63)</f>
-        <v>5538.8600000000006</v>
+        <v>0</v>
       </c>
     </row>
     <row r="65" spans="1:18">
       <c r="A65" s="21"/>
       <c r="B65" s="71" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="C65" s="72">
         <v>7.0000000000000007E-2</v>
@@ -6410,19 +5664,18 @@
       <c r="H65" s="12"/>
       <c r="I65" s="12"/>
       <c r="J65" s="12">
-        <f>ROUND(J64*C65+40,2)</f>
-        <v>184.94</v>
+        <v>0</v>
       </c>
       <c r="K65" s="12"/>
       <c r="L65" s="12">
         <f>J65</f>
-        <v>184.94</v>
+        <v>0</v>
       </c>
     </row>
     <row r="66" spans="1:18">
       <c r="A66" s="73"/>
       <c r="B66" s="74" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C66" s="63"/>
       <c r="D66" s="12"/>
@@ -6432,25 +5685,25 @@
       <c r="H66" s="12"/>
       <c r="I66" s="75">
         <f>I65+I64</f>
-        <v>2883.3699999999994</v>
+        <v>0</v>
       </c>
       <c r="J66" s="75">
         <f>J65+J64</f>
-        <v>2255.5099999999998</v>
+        <v>0</v>
       </c>
       <c r="K66" s="75">
         <f>K65+K64</f>
-        <v>584.92000000000007</v>
+        <v>0</v>
       </c>
       <c r="L66" s="75">
         <f>L65+L64</f>
-        <v>5723.8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="67" spans="1:18">
       <c r="A67" s="21"/>
       <c r="B67" s="22" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="C67" s="72">
         <v>0.09</v>
@@ -6465,13 +5718,13 @@
       <c r="K67" s="20"/>
       <c r="L67" s="20">
         <f>ROUND(L66*C67,2)</f>
-        <v>515.14</v>
+        <v>0</v>
       </c>
     </row>
     <row r="68" spans="1:18">
       <c r="A68" s="21"/>
       <c r="B68" s="22" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="C68" s="72">
         <v>7.0000000000000007E-2</v>
@@ -6486,13 +5739,13 @@
       <c r="K68" s="20"/>
       <c r="L68" s="20">
         <f>ROUND(L66*C68,2)</f>
-        <v>400.67</v>
+        <v>0</v>
       </c>
     </row>
     <row r="69" spans="1:18">
       <c r="A69" s="21"/>
       <c r="B69" s="22" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C69" s="76">
         <v>0.2359</v>
@@ -6504,19 +5757,19 @@
       <c r="H69" s="20"/>
       <c r="I69" s="20">
         <f>ROUND(I66*C69,2)</f>
-        <v>680.19</v>
+        <v>0</v>
       </c>
       <c r="J69" s="20"/>
       <c r="K69" s="20"/>
       <c r="L69" s="20">
         <f>SUM(I69:K69)</f>
-        <v>680.19</v>
+        <v>0</v>
       </c>
     </row>
     <row r="70" spans="1:18">
       <c r="A70" s="67"/>
       <c r="B70" s="68" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="C70" s="70"/>
       <c r="D70" s="69"/>
@@ -6529,13 +5782,13 @@
       <c r="K70" s="69"/>
       <c r="L70" s="69">
         <f>SUM(L66:L69)</f>
-        <v>7319.8000000000011</v>
+        <v>0</v>
       </c>
     </row>
     <row r="71" spans="1:18">
       <c r="A71" s="21"/>
       <c r="B71" s="22" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C71" s="76">
         <v>0.21</v>
@@ -6550,13 +5803,13 @@
       <c r="K71" s="20"/>
       <c r="L71" s="20">
         <f>ROUND(L70*C71,2)</f>
-        <v>1537.16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="72" spans="1:18">
       <c r="A72" s="21"/>
       <c r="B72" s="22" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C72" s="76"/>
       <c r="D72" s="20"/>
@@ -6569,7 +5822,7 @@
       <c r="K72" s="20"/>
       <c r="L72" s="20">
         <f>L70+L71</f>
-        <v>8856.9600000000009</v>
+        <v>0</v>
       </c>
     </row>
     <row r="73" spans="1:18">
@@ -6589,7 +5842,7 @@
     <row r="74" spans="1:18">
       <c r="A74" s="64"/>
       <c r="B74" s="24" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="C74" s="24"/>
       <c r="D74" s="24"/>
@@ -6605,7 +5858,7 @@
     <row r="75" spans="1:18">
       <c r="A75" s="64"/>
       <c r="B75" s="84" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="C75" s="84"/>
       <c r="D75" s="85"/>
@@ -6621,7 +5874,7 @@
     <row r="76" spans="1:18">
       <c r="A76" s="64"/>
       <c r="B76" s="84" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="C76" s="84"/>
       <c r="D76" s="85"/>
@@ -6637,7 +5890,7 @@
     <row r="77" spans="1:18">
       <c r="A77" s="64"/>
       <c r="B77" s="84" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="C77" s="84"/>
       <c r="D77" s="85"/>
@@ -6653,7 +5906,7 @@
     <row r="78" spans="1:18">
       <c r="A78" s="64"/>
       <c r="B78" s="84" t="s">
-        <v>96</v>
+        <v>44</v>
       </c>
       <c r="C78" s="84"/>
       <c r="D78" s="85"/>
@@ -6705,9 +5958,9 @@
       <c r="Q80" s="64"/>
       <c r="R80" s="64"/>
     </row>
-    <row r="81" spans="2:8" ht="15.75">
+    <row r="81" spans="2:8" ht="16">
       <c r="B81" s="89" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="H81" s="49" t="s">
         <v>4</v>
@@ -6717,18 +5970,18 @@
       <c r="B82"/>
       <c r="H82" s="43"/>
     </row>
-    <row r="83" spans="2:8" ht="15.75">
+    <row r="83" spans="2:8" ht="16">
       <c r="B83" s="89" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="H83" s="44"/>
     </row>
-    <row r="84" spans="2:8" ht="15.75">
+    <row r="84" spans="2:8" ht="16">
       <c r="B84" s="89" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="H84" s="81" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -6763,29 +6016,39 @@
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B50">
-    <cfRule type="expression" priority="27" stopIfTrue="1">
+  <conditionalFormatting sqref="B50:B51">
+    <cfRule type="expression" priority="26" stopIfTrue="1">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B59">
-    <cfRule type="expression" priority="221" stopIfTrue="1">
+  <conditionalFormatting sqref="B55">
+    <cfRule type="expression" priority="8" stopIfTrue="1">
+      <formula>#REF!</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B57:B59">
+    <cfRule type="expression" priority="1" stopIfTrue="1">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E27:F28">
-    <cfRule type="expression" priority="36" stopIfTrue="1">
-      <formula>$F$2441</formula>
+    <cfRule type="expression" priority="40" stopIfTrue="1">
+      <formula>$F$2392</formula>
     </cfRule>
     <cfRule type="expression" priority="38" stopIfTrue="1">
       <formula>$F$2488</formula>
     </cfRule>
-    <cfRule type="expression" priority="40" stopIfTrue="1">
-      <formula>$F$2392</formula>
+    <cfRule type="expression" priority="36" stopIfTrue="1">
+      <formula>$F$2441</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E50:F50">
     <cfRule type="expression" priority="28" stopIfTrue="1">
+      <formula>$F$1896</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E57:F57">
+    <cfRule type="expression" priority="4" stopIfTrue="1">
       <formula>$F$1896</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6817,6 +6080,21 @@
       <formula>$H$2791</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="F52:F53">
+    <cfRule type="expression" priority="16" stopIfTrue="1">
+      <formula>$H$2791</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F56">
+    <cfRule type="expression" priority="6" stopIfTrue="1">
+      <formula>$H$2791</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F58">
+    <cfRule type="expression" priority="2" stopIfTrue="1">
+      <formula>#REF!</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="F83">
     <cfRule type="expression" priority="475" stopIfTrue="1">
       <formula>$G$2775</formula>
@@ -6834,6 +6112,11 @@
   </conditionalFormatting>
   <conditionalFormatting sqref="G50">
     <cfRule type="expression" priority="29" stopIfTrue="1">
+      <formula>$F$1867</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G57">
+    <cfRule type="expression" priority="5" stopIfTrue="1">
       <formula>$F$1867</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6872,69 +6155,14 @@
       <formula>$H$2791</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B51">
-    <cfRule type="expression" priority="26" stopIfTrue="1">
-      <formula>#REF!</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F52">
-    <cfRule type="expression" priority="19" stopIfTrue="1">
-      <formula>$H$2791</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F53">
-    <cfRule type="expression" priority="16" stopIfTrue="1">
-      <formula>$H$2791</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I52:L52">
-    <cfRule type="expression" priority="20" stopIfTrue="1">
-      <formula>$H$2791</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I53:L53">
+  <conditionalFormatting sqref="I52:L53">
     <cfRule type="expression" priority="17" stopIfTrue="1">
       <formula>$H$2791</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B55">
-    <cfRule type="expression" priority="8" stopIfTrue="1">
-      <formula>#REF!</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B57">
-    <cfRule type="expression" priority="3" stopIfTrue="1">
-      <formula>#REF!</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E57:F57">
-    <cfRule type="expression" priority="4" stopIfTrue="1">
-      <formula>$F$1896</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F56">
-    <cfRule type="expression" priority="6" stopIfTrue="1">
-      <formula>$H$2791</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G57">
-    <cfRule type="expression" priority="5" stopIfTrue="1">
-      <formula>$F$1867</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I56:L56">
     <cfRule type="expression" priority="7" stopIfTrue="1">
       <formula>$H$2791</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B58">
-    <cfRule type="expression" priority="1" stopIfTrue="1">
-      <formula>#REF!</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F58">
-    <cfRule type="expression" priority="2" stopIfTrue="1">
-      <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <printOptions horizontalCentered="1"/>

</xml_diff>